<commit_message>
Add excel importation support for students and evaluations
</commit_message>
<xml_diff>
--- a/Eleves.xlsx
+++ b/Eleves.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\leyma\OneDrive\Documents\Cours\SAE\fast-notes\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Leymat Nicolas\Documents\GitLabCours\ProjetTuteuré\New folder\fast-notes\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{CF09F8B1-4716-41F7-B650-F97CD6A59341}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{393F5C5C-D1AA-4180-8F83-4F62AD850F54}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{04DD540D-D209-47D7-A60B-CEAFD6082BC8}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{04DD540D-D209-47D7-A60B-CEAFD6082BC8}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="24">
   <si>
     <t>Code</t>
   </si>
@@ -54,13 +54,67 @@
   </si>
   <si>
     <t>Groupe</t>
+  </si>
+  <si>
+    <t>test1</t>
+  </si>
+  <si>
+    <t>test2</t>
+  </si>
+  <si>
+    <t>test3</t>
+  </si>
+  <si>
+    <t>test4</t>
+  </si>
+  <si>
+    <t>test5</t>
+  </si>
+  <si>
+    <t>test6</t>
+  </si>
+  <si>
+    <t>test7</t>
+  </si>
+  <si>
+    <t>test8</t>
+  </si>
+  <si>
+    <t>test9</t>
+  </si>
+  <si>
+    <t>test10</t>
+  </si>
+  <si>
+    <t>test11</t>
+  </si>
+  <si>
+    <t>test12</t>
+  </si>
+  <si>
+    <t>test13</t>
+  </si>
+  <si>
+    <t>test14</t>
+  </si>
+  <si>
+    <t>test15</t>
+  </si>
+  <si>
+    <t>test16</t>
+  </si>
+  <si>
+    <t>test17</t>
+  </si>
+  <si>
+    <t>test18</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -72,6 +126,12 @@
       <b/>
       <sz val="16"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -118,7 +178,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Thème Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -414,19 +474,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{761DC1A1-87CF-4EEC-8630-3B548B9394FE}">
-  <dimension ref="A1:F1"/>
+  <dimension ref="A1:F19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="E2" sqref="E2:E19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="19.28515625" customWidth="1"/>
-    <col min="2" max="2" width="19.140625" customWidth="1"/>
+    <col min="1" max="1" width="19.33203125" customWidth="1"/>
+    <col min="2" max="2" width="19.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="21" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:6" ht="21" x14ac:dyDescent="0.4">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -446,7 +506,386 @@
         <v>5</v>
       </c>
     </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E2" t="s">
+        <v>6</v>
+      </c>
+      <c r="F2">
+        <f ca="1">RANDBETWEEN(1,3)</f>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D3" t="s">
+        <v>7</v>
+      </c>
+      <c r="E3" t="s">
+        <v>7</v>
+      </c>
+      <c r="F3">
+        <f t="shared" ref="F3:F19" ca="1" si="0">RANDBETWEEN(1,3)</f>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C4" t="s">
+        <v>8</v>
+      </c>
+      <c r="D4" t="s">
+        <v>8</v>
+      </c>
+      <c r="E4" t="s">
+        <v>8</v>
+      </c>
+      <c r="F4">
+        <f t="shared" ca="1" si="0"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>9</v>
+      </c>
+      <c r="B5" t="s">
+        <v>9</v>
+      </c>
+      <c r="C5" t="s">
+        <v>9</v>
+      </c>
+      <c r="D5" t="s">
+        <v>9</v>
+      </c>
+      <c r="E5" t="s">
+        <v>9</v>
+      </c>
+      <c r="F5">
+        <f t="shared" ca="1" si="0"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>10</v>
+      </c>
+      <c r="B6" t="s">
+        <v>10</v>
+      </c>
+      <c r="C6" t="s">
+        <v>10</v>
+      </c>
+      <c r="D6" t="s">
+        <v>10</v>
+      </c>
+      <c r="E6" t="s">
+        <v>10</v>
+      </c>
+      <c r="F6">
+        <f t="shared" ca="1" si="0"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>11</v>
+      </c>
+      <c r="B7" t="s">
+        <v>11</v>
+      </c>
+      <c r="C7" t="s">
+        <v>11</v>
+      </c>
+      <c r="D7" t="s">
+        <v>11</v>
+      </c>
+      <c r="E7" t="s">
+        <v>11</v>
+      </c>
+      <c r="F7">
+        <f t="shared" ca="1" si="0"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>12</v>
+      </c>
+      <c r="B8" t="s">
+        <v>12</v>
+      </c>
+      <c r="C8" t="s">
+        <v>12</v>
+      </c>
+      <c r="D8" t="s">
+        <v>12</v>
+      </c>
+      <c r="E8" t="s">
+        <v>12</v>
+      </c>
+      <c r="F8">
+        <f t="shared" ca="1" si="0"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>13</v>
+      </c>
+      <c r="B9" t="s">
+        <v>13</v>
+      </c>
+      <c r="C9" t="s">
+        <v>13</v>
+      </c>
+      <c r="D9" t="s">
+        <v>13</v>
+      </c>
+      <c r="E9" t="s">
+        <v>13</v>
+      </c>
+      <c r="F9">
+        <f t="shared" ca="1" si="0"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>14</v>
+      </c>
+      <c r="B10" t="s">
+        <v>14</v>
+      </c>
+      <c r="C10" t="s">
+        <v>14</v>
+      </c>
+      <c r="D10" t="s">
+        <v>14</v>
+      </c>
+      <c r="E10" t="s">
+        <v>14</v>
+      </c>
+      <c r="F10">
+        <f t="shared" ca="1" si="0"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>15</v>
+      </c>
+      <c r="B11" t="s">
+        <v>15</v>
+      </c>
+      <c r="C11" t="s">
+        <v>15</v>
+      </c>
+      <c r="D11" t="s">
+        <v>15</v>
+      </c>
+      <c r="E11" t="s">
+        <v>15</v>
+      </c>
+      <c r="F11">
+        <f t="shared" ca="1" si="0"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>16</v>
+      </c>
+      <c r="B12" t="s">
+        <v>16</v>
+      </c>
+      <c r="C12" t="s">
+        <v>16</v>
+      </c>
+      <c r="D12" t="s">
+        <v>16</v>
+      </c>
+      <c r="E12" t="s">
+        <v>16</v>
+      </c>
+      <c r="F12">
+        <f t="shared" ca="1" si="0"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>17</v>
+      </c>
+      <c r="B13" t="s">
+        <v>17</v>
+      </c>
+      <c r="C13" t="s">
+        <v>17</v>
+      </c>
+      <c r="D13" t="s">
+        <v>17</v>
+      </c>
+      <c r="E13" t="s">
+        <v>17</v>
+      </c>
+      <c r="F13">
+        <f t="shared" ca="1" si="0"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>18</v>
+      </c>
+      <c r="B14" t="s">
+        <v>18</v>
+      </c>
+      <c r="C14" t="s">
+        <v>18</v>
+      </c>
+      <c r="D14" t="s">
+        <v>18</v>
+      </c>
+      <c r="E14" t="s">
+        <v>18</v>
+      </c>
+      <c r="F14">
+        <f t="shared" ca="1" si="0"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>19</v>
+      </c>
+      <c r="B15" t="s">
+        <v>19</v>
+      </c>
+      <c r="C15" t="s">
+        <v>19</v>
+      </c>
+      <c r="D15" t="s">
+        <v>19</v>
+      </c>
+      <c r="E15" t="s">
+        <v>19</v>
+      </c>
+      <c r="F15">
+        <f t="shared" ca="1" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>20</v>
+      </c>
+      <c r="B16" t="s">
+        <v>20</v>
+      </c>
+      <c r="C16" t="s">
+        <v>20</v>
+      </c>
+      <c r="D16" t="s">
+        <v>20</v>
+      </c>
+      <c r="E16" t="s">
+        <v>20</v>
+      </c>
+      <c r="F16">
+        <f t="shared" ca="1" si="0"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
+        <v>21</v>
+      </c>
+      <c r="B17" t="s">
+        <v>21</v>
+      </c>
+      <c r="C17" t="s">
+        <v>21</v>
+      </c>
+      <c r="D17" t="s">
+        <v>21</v>
+      </c>
+      <c r="E17" t="s">
+        <v>21</v>
+      </c>
+      <c r="F17">
+        <f t="shared" ca="1" si="0"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
+        <v>22</v>
+      </c>
+      <c r="B18" t="s">
+        <v>22</v>
+      </c>
+      <c r="C18" t="s">
+        <v>22</v>
+      </c>
+      <c r="D18" t="s">
+        <v>22</v>
+      </c>
+      <c r="E18" t="s">
+        <v>22</v>
+      </c>
+      <c r="F18">
+        <f t="shared" ca="1" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
+        <v>23</v>
+      </c>
+      <c r="B19" t="s">
+        <v>23</v>
+      </c>
+      <c r="C19" t="s">
+        <v>23</v>
+      </c>
+      <c r="D19" t="s">
+        <v>23</v>
+      </c>
+      <c r="E19" t="s">
+        <v>23</v>
+      </c>
+      <c r="F19">
+        <f t="shared" ca="1" si="0"/>
+        <v>3</v>
+      </c>
+    </row>
   </sheetData>
+  <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="1200" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
Ajout condition nom de sheet
</commit_message>
<xml_diff>
--- a/Eleves.xlsx
+++ b/Eleves.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\meder\Desktop\BUT\S5\fast-notes\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{12D333AA-CAD6-4524-9FFA-405847392B0E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D166E3E8-B3FC-41D5-9E19-4B3E1913369D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{04DD540D-D209-47D7-A60B-CEAFD6082BC8}"/>
   </bookViews>
   <sheets>
-    <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
+    <sheet name="INFOS-ELEVES" sheetId="1" r:id="rId1"/>
+    <sheet name="Feuil2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -438,7 +439,7 @@
   <dimension ref="A1:F3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G7" sqref="G7"/>
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -512,4 +513,18 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="1200" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{14B074E5-33DB-43A1-8AC1-C29F5F438D54}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:F2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Ajout de plusieurs années
</commit_message>
<xml_diff>
--- a/Eleves.xlsx
+++ b/Eleves.xlsx
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\meder\Desktop\BUT\S5\fast-notes\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5889C77D-CAB7-4667-AB1A-EC9BAA735693}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FDA742B3-E782-48E3-8632-7E09EB5A4E26}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{04DD540D-D209-47D7-A60B-CEAFD6082BC8}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="2" xr2:uid="{04DD540D-D209-47D7-A60B-CEAFD6082BC8}"/>
   </bookViews>
   <sheets>
     <sheet name="INFOS-ELEVES" sheetId="1" r:id="rId1"/>
     <sheet name="INFOS-ANNEES" sheetId="2" r:id="rId2"/>
+    <sheet name="INFOS-PARCOURS" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="17">
   <si>
     <t>Code</t>
   </si>
@@ -76,6 +77,18 @@
   </si>
   <si>
     <t>annee_fin</t>
+  </si>
+  <si>
+    <t>id_parcour</t>
+  </si>
+  <si>
+    <t>id_semestre</t>
+  </si>
+  <si>
+    <t>RATIO</t>
+  </si>
+  <si>
+    <t>6_2023-2024</t>
   </si>
 </sst>
 </file>
@@ -525,7 +538,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{14B074E5-33DB-43A1-8AC1-C29F5F438D54}">
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F16" sqref="F16"/>
     </sheetView>
   </sheetViews>
@@ -553,4 +566,38 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C1D6C05B-EE68-4580-A4CF-AEBCA4B3D505}">
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I9" sqref="I9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="13" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>